<commit_message>
fixed names on allgraph
</commit_message>
<xml_diff>
--- a/marbleracing/season2/scoreboard.xlsx
+++ b/marbleracing/season2/scoreboard.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>Flair</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>Race 8</t>
+  </si>
+  <si>
+    <t>MoscaMye</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>1st (+100)</t>
+  </si>
+  <si>
+    <t>Zokalyx</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>2nd (+99)</t>
   </si>
 </sst>
 </file>
@@ -75,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -103,6 +127,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="6" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
@@ -446,6 +471,44 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -453,13 +516,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="6" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
@@ -502,6 +565,44 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -509,13 +610,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="6" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
@@ -558,6 +659,44 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>